<commit_message>
Added more FCS schools to conferences spreadsheets
</commit_message>
<xml_diff>
--- a/src/main/resources/Default_06_Conferences.xlsx
+++ b/src/main/resources/Default_06_Conferences.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsbol\IdeaProjects\NCAA_06_Scheduler\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\newRepos\other\ncaa-06-scheduler\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD9611DE-AACC-4F46-A7BB-EB7413A34EE1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="Jared 06 Conferences" sheetId="2" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="279">
   <si>
     <t>TGID</t>
   </si>
@@ -789,12 +788,84 @@
   <si>
     <t>Ohio Valley</t>
   </si>
+  <si>
+    <t>Appalachian State</t>
+  </si>
+  <si>
+    <t>SoCon</t>
+  </si>
+  <si>
+    <t>The Citadel</t>
+  </si>
+  <si>
+    <t>Furman</t>
+  </si>
+  <si>
+    <t>Georgia Southern</t>
+  </si>
+  <si>
+    <t>Western Carolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catamounts </t>
+  </si>
+  <si>
+    <t>Chattanooga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mocs </t>
+  </si>
+  <si>
+    <t>Villanova</t>
+  </si>
+  <si>
+    <t>Colonial</t>
+  </si>
+  <si>
+    <t>Minutemen</t>
+  </si>
+  <si>
+    <t>James Madison</t>
+  </si>
+  <si>
+    <t>Dukes</t>
+  </si>
+  <si>
+    <t>Harvard</t>
+  </si>
+  <si>
+    <t>Crimson</t>
+  </si>
+  <si>
+    <t>Ivy League</t>
+  </si>
+  <si>
+    <t>Eastern Washington</t>
+  </si>
+  <si>
+    <t>Big Sky</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Grizzlies</t>
+  </si>
+  <si>
+    <t>Hilltoppers</t>
+  </si>
+  <si>
+    <t>Eastern Kentucky</t>
+  </si>
+  <si>
+    <t>Paladins</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -846,6 +917,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -892,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -984,6 +1061,15 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1298,41 +1384,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA1121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E120" sqref="E120"/>
+      <selection pane="bottomRight" activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.703125" customWidth="1"/>
-    <col min="2" max="2" width="22.703125" customWidth="1"/>
-    <col min="3" max="3" width="17.29296875" customWidth="1"/>
-    <col min="4" max="4" width="17.41015625" customWidth="1"/>
-    <col min="5" max="5" width="15.87890625" customWidth="1"/>
-    <col min="6" max="6" width="8.29296875" customWidth="1"/>
-    <col min="7" max="7" width="18.29296875" customWidth="1"/>
-    <col min="8" max="8" width="18.41015625" customWidth="1"/>
-    <col min="9" max="9" width="20.87890625" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="13.29296875" customWidth="1"/>
-    <col min="12" max="13" width="12.1171875" customWidth="1"/>
-    <col min="14" max="14" width="8.87890625" customWidth="1"/>
-    <col min="15" max="15" width="10.703125" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
     <col min="16" max="17" width="12" customWidth="1"/>
-    <col min="18" max="33" width="9.1171875" customWidth="1"/>
-    <col min="34" max="34" width="11.29296875" customWidth="1"/>
-    <col min="35" max="36" width="9.29296875" customWidth="1"/>
-    <col min="37" max="38" width="9.1171875" customWidth="1"/>
-    <col min="39" max="40" width="9.29296875" customWidth="1"/>
-    <col min="41" max="41" width="9.87890625" customWidth="1"/>
-    <col min="42" max="44" width="9.1171875" customWidth="1"/>
-    <col min="45" max="53" width="8.703125" customWidth="1"/>
+    <col min="18" max="33" width="9.140625" customWidth="1"/>
+    <col min="34" max="34" width="11.28515625" customWidth="1"/>
+    <col min="35" max="36" width="9.28515625" customWidth="1"/>
+    <col min="37" max="38" width="9.140625" customWidth="1"/>
+    <col min="39" max="40" width="9.28515625" customWidth="1"/>
+    <col min="41" max="41" width="9.85546875" customWidth="1"/>
+    <col min="42" max="44" width="9.140625" customWidth="1"/>
+    <col min="45" max="53" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="14.25" customHeight="1">
@@ -10131,10 +10217,13 @@
       <c r="F121" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G121" s="24" t="s">
+      <c r="G121" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="H121" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="H121" s="24" t="s">
+      <c r="I121" s="24" t="s">
         <v>131</v>
       </c>
       <c r="O121" s="22"/>
@@ -10177,13 +10266,25 @@
       <c r="AZ121" s="21"/>
     </row>
     <row r="122" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A122" s="29"/>
-      <c r="B122" s="25"/>
-      <c r="C122" s="25"/>
-      <c r="D122" s="25"/>
-      <c r="E122" s="25"/>
-      <c r="F122" s="16"/>
-      <c r="G122" s="26"/>
+      <c r="A122" s="36">
+        <v>188</v>
+      </c>
+      <c r="B122" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="C122" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="D122" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="E122" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="F122" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G122" s="37"/>
       <c r="H122" s="26"/>
       <c r="I122" s="16"/>
       <c r="J122" s="16"/>
@@ -10231,13 +10332,27 @@
       <c r="AZ122" s="21"/>
     </row>
     <row r="123" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A123" s="29"/>
-      <c r="B123" s="25"/>
-      <c r="C123" s="25"/>
-      <c r="D123" s="25"/>
-      <c r="E123" s="25"/>
-      <c r="F123" s="16"/>
-      <c r="G123" s="26"/>
+      <c r="A123" s="36">
+        <v>190</v>
+      </c>
+      <c r="B123" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="C123" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="D123" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E123" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="F123" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G123" s="37" t="s">
+        <v>258</v>
+      </c>
       <c r="H123" s="26"/>
       <c r="I123" s="27"/>
       <c r="J123" s="15"/>
@@ -10285,13 +10400,25 @@
       <c r="AZ123" s="21"/>
     </row>
     <row r="124" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A124" s="29"/>
-      <c r="B124" s="25"/>
-      <c r="C124" s="25"/>
-      <c r="D124" s="25"/>
-      <c r="E124" s="25"/>
-      <c r="F124" s="16"/>
-      <c r="G124" s="26"/>
+      <c r="A124" s="36">
+        <v>193</v>
+      </c>
+      <c r="B124" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="C124" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D124" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E124" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="F124" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G124" s="37"/>
       <c r="H124" s="26"/>
       <c r="I124" s="27"/>
       <c r="J124" s="27"/>
@@ -10339,13 +10466,25 @@
       <c r="AZ124" s="21"/>
     </row>
     <row r="125" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A125" s="29"/>
-      <c r="B125" s="25"/>
-      <c r="C125" s="25"/>
-      <c r="D125" s="25"/>
-      <c r="E125" s="25"/>
-      <c r="F125" s="16"/>
-      <c r="G125" s="26"/>
+      <c r="A125" s="36">
+        <v>195</v>
+      </c>
+      <c r="B125" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="C125" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D125" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="E125" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="F125" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G125" s="37"/>
       <c r="H125" s="26"/>
       <c r="I125" s="27"/>
       <c r="J125" s="27"/>
@@ -10393,13 +10532,25 @@
       <c r="AZ125" s="21"/>
     </row>
     <row r="126" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A126" s="29"/>
-      <c r="B126" s="25"/>
-      <c r="C126" s="25"/>
-      <c r="D126" s="25"/>
-      <c r="E126" s="25"/>
-      <c r="F126" s="16"/>
-      <c r="G126" s="26"/>
+      <c r="A126" s="36">
+        <v>194</v>
+      </c>
+      <c r="B126" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="C126" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="D126" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E126" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="F126" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G126" s="37"/>
       <c r="H126" s="26"/>
       <c r="I126" s="27"/>
       <c r="J126" s="15"/>
@@ -10447,13 +10598,25 @@
       <c r="AZ126" s="21"/>
     </row>
     <row r="127" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A127" s="29"/>
-      <c r="B127" s="25"/>
-      <c r="C127" s="25"/>
-      <c r="D127" s="25"/>
-      <c r="E127" s="25"/>
-      <c r="F127" s="16"/>
-      <c r="G127" s="26"/>
+      <c r="A127" s="36">
+        <v>186</v>
+      </c>
+      <c r="B127" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="C127" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D127" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="E127" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="F127" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G127" s="37"/>
       <c r="H127" s="26"/>
       <c r="I127" s="27"/>
       <c r="J127" s="15"/>
@@ -10501,13 +10664,25 @@
       <c r="AZ127" s="21"/>
     </row>
     <row r="128" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A128" s="29"/>
-      <c r="B128" s="25"/>
-      <c r="C128" s="25"/>
-      <c r="D128" s="25"/>
-      <c r="E128" s="25"/>
-      <c r="F128" s="16"/>
-      <c r="G128" s="16"/>
+      <c r="A128" s="36">
+        <v>181</v>
+      </c>
+      <c r="B128" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C128" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="D128" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E128" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="F128" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G128" s="36"/>
       <c r="H128" s="16"/>
       <c r="I128" s="16"/>
       <c r="J128" s="16"/>
@@ -10555,13 +10730,25 @@
       <c r="AZ128" s="16"/>
     </row>
     <row r="129" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A129" s="29"/>
-      <c r="B129" s="25"/>
-      <c r="C129" s="25"/>
-      <c r="D129" s="25"/>
-      <c r="E129" s="25"/>
-      <c r="F129" s="16"/>
-      <c r="G129" s="16"/>
+      <c r="A129" s="36">
+        <v>179</v>
+      </c>
+      <c r="B129" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="C129" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="D129" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="E129" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="F129" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G129" s="36"/>
       <c r="H129" s="16"/>
       <c r="I129" s="16"/>
       <c r="J129" s="16"/>
@@ -10609,13 +10796,25 @@
       <c r="AZ129" s="16"/>
     </row>
     <row r="130" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A130" s="29"/>
-      <c r="B130" s="25"/>
-      <c r="C130" s="25"/>
-      <c r="D130" s="25"/>
-      <c r="E130" s="25"/>
-      <c r="F130" s="16"/>
-      <c r="G130" s="16"/>
+      <c r="A130" s="36">
+        <v>129</v>
+      </c>
+      <c r="B130" s="36" t="s">
+        <v>269</v>
+      </c>
+      <c r="C130" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="D130" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E130" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="F130" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G130" s="36"/>
       <c r="H130" s="16"/>
       <c r="I130" s="16"/>
       <c r="J130" s="16"/>
@@ -10663,13 +10862,25 @@
       <c r="AZ130" s="16"/>
     </row>
     <row r="131" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A131" s="29"/>
-      <c r="B131" s="25"/>
-      <c r="C131" s="25"/>
-      <c r="D131" s="25"/>
-      <c r="E131" s="25"/>
-      <c r="F131" s="16"/>
-      <c r="G131" s="16"/>
+      <c r="A131" s="36">
+        <v>197</v>
+      </c>
+      <c r="B131" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="C131" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D131" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="E131" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="F131" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G131" s="36"/>
       <c r="H131" s="16"/>
       <c r="I131" s="16"/>
       <c r="J131" s="16"/>
@@ -10717,13 +10928,25 @@
       <c r="AZ131" s="16"/>
     </row>
     <row r="132" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A132" s="29"/>
-      <c r="B132" s="25"/>
-      <c r="C132" s="25"/>
-      <c r="D132" s="25"/>
-      <c r="E132" s="25"/>
-      <c r="F132" s="16"/>
-      <c r="G132" s="16"/>
+      <c r="A132" s="36">
+        <v>199</v>
+      </c>
+      <c r="B132" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="C132" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="D132" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="E132" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="F132" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G132" s="36"/>
       <c r="H132" s="16"/>
       <c r="I132" s="16"/>
       <c r="J132" s="16"/>
@@ -10771,13 +10994,27 @@
       <c r="AZ132" s="16"/>
     </row>
     <row r="133" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A133" s="29"/>
-      <c r="B133" s="25"/>
-      <c r="C133" s="25"/>
-      <c r="D133" s="25"/>
-      <c r="E133" s="25"/>
-      <c r="F133" s="16"/>
-      <c r="G133" s="16"/>
+      <c r="A133" s="36">
+        <v>211</v>
+      </c>
+      <c r="B133" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="C133" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="D133" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="E133" s="36" t="s">
+        <v>254</v>
+      </c>
+      <c r="F133" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G133" s="36" t="s">
+        <v>277</v>
+      </c>
       <c r="H133" s="16"/>
       <c r="I133" s="16"/>
       <c r="J133" s="16"/>
@@ -10825,13 +11062,27 @@
       <c r="AZ133" s="16"/>
     </row>
     <row r="134" spans="1:52" ht="14.25" customHeight="1">
-      <c r="A134" s="29"/>
-      <c r="B134" s="25"/>
-      <c r="C134" s="25"/>
-      <c r="D134" s="25"/>
-      <c r="E134" s="25"/>
-      <c r="F134" s="16"/>
-      <c r="G134" s="16"/>
+      <c r="A134" s="36">
+        <v>192</v>
+      </c>
+      <c r="B134" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="C134" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="D134" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E134" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="F134" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G134" s="36" t="s">
+        <v>257</v>
+      </c>
       <c r="H134" s="16"/>
       <c r="I134" s="16"/>
       <c r="J134" s="16"/>
@@ -35142,8 +35393,8 @@
       <c r="AZ1121" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N121" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N121">
+  <autoFilter ref="A1:N121">
+    <sortState ref="A2:N121">
       <sortCondition ref="E2:E121" customList="ACC,Big East,Big Ten,Big 12,Pac-12,Pac-10,SEC,Independent,MWC,C-USA,WAC,MAC,Sun Belt"/>
     </sortState>
   </autoFilter>

</xml_diff>